<commit_message>
menemukan cara untuk menyimpan data keyword dan mencari irisannya dengan intersect1d, data yang digunakan adalah list
</commit_message>
<xml_diff>
--- a/write_data.xlsx
+++ b/write_data.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universitas Trunojoyo Madura\#Kuliah\#SKRIPSI\dokumen\program\sv-k-modes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F770946E-222C-4DA0-8F2D-0ECBB38D44A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="11160" yWindow="1185" windowWidth="9135" windowHeight="5580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>ekonomi,moneter</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>ekonomi,mikro</t>
   </si>
@@ -25,9 +28,6 @@
     <t>ekonomi</t>
   </si>
   <si>
-    <t>coreldraw</t>
-  </si>
-  <si>
     <t>kepemimpinan,organisasi</t>
   </si>
   <si>
@@ -37,17 +37,35 @@
     <t>sekolah,jaringan</t>
   </si>
   <si>
-    <t>kepemimpinan,sekolah,budayamutu</t>
-  </si>
-  <si>
     <t>komunikasi,manusia</t>
+  </si>
+  <si>
+    <t>corel draw</t>
+  </si>
+  <si>
+    <t>kepemimpinan,sekolah,budaya mutu</t>
+  </si>
+  <si>
+    <t>kepemimpinan</t>
+  </si>
+  <si>
+    <t>manusia</t>
+  </si>
+  <si>
+    <t>sekolah</t>
+  </si>
+  <si>
+    <t>komunikasi</t>
+  </si>
+  <si>
+    <t>moneter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +102,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -130,7 +156,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -162,9 +188,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -196,6 +240,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -371,83 +433,116 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
penyelesaian GICCA sebelum menggunakan class
</commit_message>
<xml_diff>
--- a/write_data.xlsx
+++ b/write_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universitas Trunojoyo Madura\#Kuliah\#SKRIPSI\dokumen\program\sv-k-modes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F770946E-222C-4DA0-8F2D-0ECBB38D44A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E6F992-BF5C-459D-A031-5EC06DF95BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="1185" windowWidth="9135" windowHeight="5580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8790" yWindow="465" windowWidth="10470" windowHeight="5625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>ekonomi,mikro</t>
   </si>
@@ -43,22 +43,10 @@
     <t>corel draw</t>
   </si>
   <si>
-    <t>kepemimpinan,sekolah,budaya mutu</t>
-  </si>
-  <si>
-    <t>kepemimpinan</t>
-  </si>
-  <si>
-    <t>manusia</t>
-  </si>
-  <si>
-    <t>sekolah</t>
-  </si>
-  <si>
-    <t>komunikasi</t>
-  </si>
-  <si>
-    <t>moneter</t>
+    <t>ekonomi,moneter</t>
+  </si>
+  <si>
+    <t>kepemimpinan,sekolah,budayamutu</t>
   </si>
 </sst>
 </file>
@@ -434,115 +422,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="36" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gicca selesai, svkmodes sudah iterasi pertama
</commit_message>
<xml_diff>
--- a/write_data.xlsx
+++ b/write_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universitas Trunojoyo Madura\#Kuliah\#SKRIPSI\dokumen\program\sv-k-modes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E6F992-BF5C-459D-A031-5EC06DF95BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3883C8-F5CD-4999-BD49-31C664DCE020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8790" yWindow="465" windowWidth="10470" windowHeight="5625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,33 +20,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>ekonomi,mikro</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>ekonomi</t>
   </si>
   <si>
-    <t>kepemimpinan,organisasi</t>
-  </si>
-  <si>
-    <t>manusia,salmon</t>
-  </si>
-  <si>
-    <t>sekolah,jaringan</t>
-  </si>
-  <si>
-    <t>komunikasi,manusia</t>
-  </si>
-  <si>
     <t>corel draw</t>
   </si>
   <si>
-    <t>ekonomi,moneter</t>
-  </si>
-  <si>
-    <t>kepemimpinan,sekolah,budayamutu</t>
+    <t>ekonomi, moneter</t>
+  </si>
+  <si>
+    <t>ekonomi, mikro</t>
+  </si>
+  <si>
+    <t>kepemimpinan, organisasi</t>
+  </si>
+  <si>
+    <t>manusia, salmon</t>
+  </si>
+  <si>
+    <t>sekolah, jaringan</t>
+  </si>
+  <si>
+    <t>kepemimpinan, sekolah, budaya mutu</t>
+  </si>
+  <si>
+    <t>komunikasi, manusia</t>
   </si>
 </sst>
 </file>
@@ -422,15 +422,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A10" sqref="A10:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -438,7 +439,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -446,7 +447,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -454,7 +455,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -462,7 +463,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -470,7 +471,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -478,7 +479,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -486,7 +487,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -494,7 +495,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -502,7 +503,47 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>